<commit_message>
Est11 Outputs for each metro area
Est11 Outputs for each metro area created. Please find them in *\Factors and Ridership Data\Script Outputs\Est11_Outputs
</commit_message>
<xml_diff>
--- a/Factors and Ridership Data/Script Outputs/Est9_Outputs/Model2/Template/template.xlsx
+++ b/Factors and Ridership Data/Script Outputs/Est9_Outputs/Model2/Template/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UoK\OneDrive - University of Kentucky\github\Transit_ridership\transit_ridership_decline\Factors and Ridership Data\Script Outputs\Est9_Outputs\Model2\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luky-my.sharepoint.com/personal/vsgo222_uky_edu/Documents/github/Transit_ridership/transit_ridership_decline/Factors and Ridership Data/Script Outputs/Est9_Outputs/Model2/Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{5FFA77E9-E419-4791-B818-B96F613B29FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5558FF72-5026-4466-9E7A-EEC23D9405CF}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{5FFA77E9-E419-4791-B818-B96F613B29FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D63C77C6-7124-4E70-B7A0-9CC2F007DA30}"/>
   <bookViews>
-    <workbookView xWindow="7050" yWindow="780" windowWidth="18855" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -860,14 +860,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>

</xml_diff>